<commit_message>
dodałem kolumnę z procentową inwestycja w dzień
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t/>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Suma godzin</t>
+  </si>
+  <si>
+    <t>Udział dnia</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -163,14 +169,16 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -178,6 +186,7 @@
   <cols>
     <col min="1" max="1" width="11.69921875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.9453125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.20703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -192,6 +201,9 @@
       <c r="B2" t="s">
         <v>33</v>
       </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -205,6 +217,9 @@
       <c r="B4" t="n" s="1">
         <v>0.0</v>
       </c>
+      <c r="C4" t="n" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -213,6 +228,9 @@
       <c r="B5" t="n" s="1">
         <v>107.0</v>
       </c>
+      <c r="C5" t="n" s="1">
+        <v>0.02069799229502678</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -221,6 +239,9 @@
       <c r="B6" t="n" s="1">
         <v>0.0</v>
       </c>
+      <c r="C6" t="n" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -229,6 +250,9 @@
       <c r="B7" t="n" s="1">
         <v>210.89999389648438</v>
       </c>
+      <c r="C7" t="n" s="1">
+        <v>0.040796320885419846</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -237,6 +261,9 @@
       <c r="B8" t="n" s="1">
         <v>177.5</v>
       </c>
+      <c r="C8" t="n" s="1">
+        <v>0.03433545306324959</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -245,6 +272,9 @@
       <c r="B9" t="n" s="1">
         <v>206.0</v>
       </c>
+      <c r="C9" t="n" s="1">
+        <v>0.03984847292304039</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -253,6 +283,9 @@
       <c r="B10" t="n" s="1">
         <v>215.39999389648438</v>
       </c>
+      <c r="C10" t="n" s="1">
+        <v>0.041666798293590546</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -261,6 +294,9 @@
       <c r="B11" t="n" s="1">
         <v>201.1999969482422</v>
       </c>
+      <c r="C11" t="n" s="1">
+        <v>0.03891996294260025</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -269,6 +305,9 @@
       <c r="B12" t="n" s="1">
         <v>156.0</v>
       </c>
+      <c r="C12" t="n" s="1">
+        <v>0.030176512897014618</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -277,6 +316,9 @@
       <c r="B13" t="n" s="1">
         <v>0.0</v>
       </c>
+      <c r="C13" t="n" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -285,6 +327,9 @@
       <c r="B14" t="n" s="1">
         <v>222.5</v>
       </c>
+      <c r="C14" t="n" s="1">
+        <v>0.04304021969437599</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -293,6 +338,9 @@
       <c r="B15" t="n" s="1">
         <v>190.0</v>
       </c>
+      <c r="C15" t="n" s="1">
+        <v>0.036753445863723755</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -301,6 +349,9 @@
       <c r="B16" t="n" s="1">
         <v>191.5</v>
       </c>
+      <c r="C16" t="n" s="1">
+        <v>0.037043604999780655</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -309,6 +360,9 @@
       <c r="B17" t="n" s="1">
         <v>195.5</v>
       </c>
+      <c r="C17" t="n" s="1">
+        <v>0.03781735897064209</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -317,6 +371,9 @@
       <c r="B18" t="n" s="1">
         <v>199.5</v>
       </c>
+      <c r="C18" t="n" s="1">
+        <v>0.03859111666679382</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -325,6 +382,9 @@
       <c r="B19" t="n" s="1">
         <v>250.0</v>
       </c>
+      <c r="C19" t="n" s="1">
+        <v>0.04835979640483856</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -333,6 +393,9 @@
       <c r="B20" t="n" s="1">
         <v>0.0</v>
       </c>
+      <c r="C20" t="n" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -341,6 +404,9 @@
       <c r="B21" t="n" s="1">
         <v>255.0</v>
       </c>
+      <c r="C21" t="n" s="1">
+        <v>0.04932698979973793</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -349,6 +415,9 @@
       <c r="B22" t="n" s="1">
         <v>174.0</v>
       </c>
+      <c r="C22" t="n" s="1">
+        <v>0.03365841880440712</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -357,6 +426,9 @@
       <c r="B23" t="n" s="1">
         <v>186.0</v>
       </c>
+      <c r="C23" t="n" s="1">
+        <v>0.03597968816757202</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -365,6 +437,9 @@
       <c r="B24" t="n" s="1">
         <v>201.5</v>
       </c>
+      <c r="C24" t="n" s="1">
+        <v>0.03897799551486969</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -373,6 +448,9 @@
       <c r="B25" t="n" s="1">
         <v>217.0</v>
       </c>
+      <c r="C25" t="n" s="1">
+        <v>0.04197630286216736</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -381,6 +459,9 @@
       <c r="B26" t="n" s="1">
         <v>239.5</v>
       </c>
+      <c r="C26" t="n" s="1">
+        <v>0.04632868245244026</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -389,6 +470,9 @@
       <c r="B27" t="n" s="1">
         <v>0.0</v>
       </c>
+      <c r="C27" t="n" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -397,6 +481,9 @@
       <c r="B28" t="n" s="1">
         <v>231.0</v>
       </c>
+      <c r="C28" t="n" s="1">
+        <v>0.04468445107340813</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -405,6 +492,9 @@
       <c r="B29" t="n" s="1">
         <v>207.0</v>
       </c>
+      <c r="C29" t="n" s="1">
+        <v>0.04004191234707832</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -413,6 +503,9 @@
       <c r="B30" t="n" s="1">
         <v>189.5</v>
       </c>
+      <c r="C30" t="n" s="1">
+        <v>0.03665672615170479</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
@@ -421,6 +514,9 @@
       <c r="B31" t="n" s="1">
         <v>196.60000610351562</v>
       </c>
+      <c r="C31" t="n" s="1">
+        <v>0.038030143827199936</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -429,6 +525,9 @@
       <c r="B32" t="n" s="1">
         <v>264.48333740234375</v>
       </c>
+      <c r="C32" t="n" s="1">
+        <v>0.05116144195199013</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -437,6 +536,9 @@
       <c r="B33" t="n" s="1">
         <v>285.0</v>
       </c>
+      <c r="C33" t="n" s="1">
+        <v>0.055130165070295334</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
@@ -445,10 +547,16 @@
       <c r="B34" t="n" s="1">
         <v>0.0</v>
       </c>
+      <c r="C34" t="n" s="1">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" t="n" s="2">
         <v>5169.58349609375</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ForecastReader, and method to write it to report. It is bugged.
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t/>
   </si>
@@ -120,6 +120,102 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Pilotaż obrotu</t>
+  </si>
+  <si>
+    <t>126669</t>
+  </si>
+  <si>
+    <t>124994</t>
+  </si>
+  <si>
+    <t>99470</t>
+  </si>
+  <si>
+    <t>4770</t>
+  </si>
+  <si>
+    <t>137076</t>
+  </si>
+  <si>
+    <t>130174</t>
+  </si>
+  <si>
+    <t>264911</t>
+  </si>
+  <si>
+    <t>888064</t>
+  </si>
+  <si>
+    <t>7125</t>
+  </si>
+  <si>
+    <t>11106</t>
+  </si>
+  <si>
+    <t>140474</t>
+  </si>
+  <si>
+    <t>142267</t>
+  </si>
+  <si>
+    <t>133568</t>
+  </si>
+  <si>
+    <t>153107</t>
+  </si>
+  <si>
+    <t>256672</t>
+  </si>
+  <si>
+    <t>844319</t>
+  </si>
+  <si>
+    <t>7840</t>
+  </si>
+  <si>
+    <t>136106</t>
+  </si>
+  <si>
+    <t>121366</t>
+  </si>
+  <si>
+    <t>113134</t>
+  </si>
+  <si>
+    <t>121171</t>
+  </si>
+  <si>
+    <t>115064</t>
+  </si>
+  <si>
+    <t>169608</t>
+  </si>
+  <si>
+    <t>784289</t>
+  </si>
+  <si>
+    <t>10002</t>
+  </si>
+  <si>
+    <t>85496</t>
+  </si>
+  <si>
+    <t>73450</t>
+  </si>
+  <si>
+    <t>74707</t>
+  </si>
+  <si>
+    <t>68280</t>
+  </si>
+  <si>
+    <t>76074</t>
+  </si>
+  <si>
+    <t>115731</t>
   </si>
 </sst>
 </file>
@@ -180,7 +276,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -189,6 +285,7 @@
     <col min="1" max="1" width="11.69921875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.9453125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.20703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.71875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -206,6 +303,9 @@
       <c r="C2" t="s">
         <v>34</v>
       </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -222,6 +322,9 @@
       <c r="C4" t="n" s="3">
         <v>0.0</v>
       </c>
+      <c r="D4" t="s" s="1">
+        <v>37</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -233,6 +336,9 @@
       <c r="C5" t="n" s="3">
         <v>0.02069799229502678</v>
       </c>
+      <c r="D5" t="s" s="1">
+        <v>38</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -244,6 +350,9 @@
       <c r="C6" t="n" s="3">
         <v>0.0</v>
       </c>
+      <c r="D6" t="s" s="1">
+        <v>39</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -255,6 +364,9 @@
       <c r="C7" t="n" s="3">
         <v>0.040796320885419846</v>
       </c>
+      <c r="D7" t="s" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -266,6 +378,9 @@
       <c r="C8" t="n" s="3">
         <v>0.03433545306324959</v>
       </c>
+      <c r="D8" t="s" s="1">
+        <v>41</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -277,6 +392,9 @@
       <c r="C9" t="n" s="3">
         <v>0.03984847292304039</v>
       </c>
+      <c r="D9" t="s" s="1">
+        <v>42</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -288,6 +406,9 @@
       <c r="C10" t="n" s="3">
         <v>0.041666798293590546</v>
       </c>
+      <c r="D10" t="s" s="1">
+        <v>43</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -299,6 +420,9 @@
       <c r="C11" t="n" s="3">
         <v>0.03891996294260025</v>
       </c>
+      <c r="D11" t="s" s="1">
+        <v>44</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -310,6 +434,9 @@
       <c r="C12" t="n" s="3">
         <v>0.030176512897014618</v>
       </c>
+      <c r="D12" t="s" s="1">
+        <v>45</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -321,6 +448,9 @@
       <c r="C13" t="n" s="3">
         <v>0.0</v>
       </c>
+      <c r="D13" t="s" s="1">
+        <v>46</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -332,6 +462,9 @@
       <c r="C14" t="n" s="3">
         <v>0.04304021969437599</v>
       </c>
+      <c r="D14" t="s" s="1">
+        <v>47</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -343,6 +476,9 @@
       <c r="C15" t="n" s="3">
         <v>0.036753445863723755</v>
       </c>
+      <c r="D15" t="s" s="1">
+        <v>48</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -354,6 +490,9 @@
       <c r="C16" t="n" s="3">
         <v>0.037043604999780655</v>
       </c>
+      <c r="D16" t="s" s="1">
+        <v>49</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -365,6 +504,9 @@
       <c r="C17" t="n" s="3">
         <v>0.03781735897064209</v>
       </c>
+      <c r="D17" t="s" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -376,6 +518,9 @@
       <c r="C18" t="n" s="3">
         <v>0.03859111666679382</v>
       </c>
+      <c r="D18" t="s" s="1">
+        <v>51</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -387,6 +532,9 @@
       <c r="C19" t="n" s="3">
         <v>0.04835979640483856</v>
       </c>
+      <c r="D19" t="s" s="1">
+        <v>52</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -398,6 +546,9 @@
       <c r="C20" t="n" s="3">
         <v>0.0</v>
       </c>
+      <c r="D20" t="s" s="1">
+        <v>53</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -409,6 +560,9 @@
       <c r="C21" t="n" s="3">
         <v>0.04932698979973793</v>
       </c>
+      <c r="D21" t="s" s="1">
+        <v>54</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -420,6 +574,9 @@
       <c r="C22" t="n" s="3">
         <v>0.03365841880440712</v>
       </c>
+      <c r="D22" t="s" s="1">
+        <v>55</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -431,6 +588,9 @@
       <c r="C23" t="n" s="3">
         <v>0.03597968816757202</v>
       </c>
+      <c r="D23" t="s" s="1">
+        <v>56</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -442,6 +602,9 @@
       <c r="C24" t="n" s="3">
         <v>0.03897799551486969</v>
       </c>
+      <c r="D24" t="s" s="1">
+        <v>57</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -453,6 +616,9 @@
       <c r="C25" t="n" s="3">
         <v>0.04197630286216736</v>
       </c>
+      <c r="D25" t="s" s="1">
+        <v>58</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -464,6 +630,9 @@
       <c r="C26" t="n" s="3">
         <v>0.04632868245244026</v>
       </c>
+      <c r="D26" t="s" s="1">
+        <v>59</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -475,6 +644,9 @@
       <c r="C27" t="n" s="3">
         <v>0.0</v>
       </c>
+      <c r="D27" t="s" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -486,6 +658,9 @@
       <c r="C28" t="n" s="3">
         <v>0.04468445107340813</v>
       </c>
+      <c r="D28" t="s" s="1">
+        <v>61</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -497,6 +672,9 @@
       <c r="C29" t="n" s="3">
         <v>0.04004191234707832</v>
       </c>
+      <c r="D29" t="s" s="1">
+        <v>62</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -508,6 +686,9 @@
       <c r="C30" t="n" s="3">
         <v>0.03665672615170479</v>
       </c>
+      <c r="D30" t="s" s="1">
+        <v>63</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
@@ -519,6 +700,9 @@
       <c r="C31" t="n" s="3">
         <v>0.038030143827199936</v>
       </c>
+      <c r="D31" t="s" s="1">
+        <v>64</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -530,6 +714,9 @@
       <c r="C32" t="n" s="3">
         <v>0.05116144195199013</v>
       </c>
+      <c r="D32" t="s" s="1">
+        <v>65</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -541,6 +728,9 @@
       <c r="C33" t="n" s="3">
         <v>0.055130165070295334</v>
       </c>
+      <c r="D33" t="s" s="1">
+        <v>66</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
@@ -551,6 +741,9 @@
       </c>
       <c r="C34" t="n" s="3">
         <v>0.0</v>
+      </c>
+      <c r="D34" t="s" s="1">
+        <v>67</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
nullPointer Ex in ForecastReader was taken care of.
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -146,9 +146,6 @@
     <t>264911</t>
   </si>
   <si>
-    <t>888064</t>
-  </si>
-  <si>
     <t>7125</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>256672</t>
   </si>
   <si>
-    <t>844319</t>
-  </si>
-  <si>
     <t>7840</t>
   </si>
   <si>
@@ -194,9 +188,6 @@
     <t>169608</t>
   </si>
   <si>
-    <t>784289</t>
-  </si>
-  <si>
     <t>10002</t>
   </si>
   <si>
@@ -216,6 +207,15 @@
   </si>
   <si>
     <t>115731</t>
+  </si>
+  <si>
+    <t>92381</t>
+  </si>
+  <si>
+    <t>72400</t>
+  </si>
+  <si>
+    <t>61582</t>
   </si>
 </sst>
 </file>
@@ -282,10 +282,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.69921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.9453125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.20703125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.71875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.3046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.39453125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.9453125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
class MonthChecker added, which check which month is to be reported. ReportWriter now write only forecasted Turn Over from desired month.
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t/>
   </si>
@@ -125,97 +125,70 @@
     <t>Pilotaż obrotu</t>
   </si>
   <si>
-    <t>126669</t>
-  </si>
-  <si>
-    <t>124994</t>
-  </si>
-  <si>
-    <t>99470</t>
-  </si>
-  <si>
-    <t>4770</t>
-  </si>
-  <si>
-    <t>137076</t>
-  </si>
-  <si>
-    <t>130174</t>
-  </si>
-  <si>
-    <t>264911</t>
-  </si>
-  <si>
-    <t>7125</t>
-  </si>
-  <si>
-    <t>11106</t>
-  </si>
-  <si>
-    <t>140474</t>
-  </si>
-  <si>
-    <t>142267</t>
-  </si>
-  <si>
-    <t>133568</t>
-  </si>
-  <si>
-    <t>153107</t>
-  </si>
-  <si>
-    <t>256672</t>
-  </si>
-  <si>
-    <t>7840</t>
-  </si>
-  <si>
-    <t>136106</t>
-  </si>
-  <si>
-    <t>121366</t>
-  </si>
-  <si>
-    <t>113134</t>
-  </si>
-  <si>
-    <t>121171</t>
-  </si>
-  <si>
-    <t>115064</t>
-  </si>
-  <si>
-    <t>169608</t>
-  </si>
-  <si>
-    <t>10002</t>
-  </si>
-  <si>
-    <t>85496</t>
-  </si>
-  <si>
-    <t>73450</t>
-  </si>
-  <si>
-    <t>74707</t>
-  </si>
-  <si>
-    <t>68280</t>
-  </si>
-  <si>
-    <t>76074</t>
-  </si>
-  <si>
-    <t>115731</t>
-  </si>
-  <si>
-    <t>92381</t>
-  </si>
-  <si>
-    <t>72400</t>
-  </si>
-  <si>
-    <t>61582</t>
+    <t>25832</t>
+  </si>
+  <si>
+    <t>37363</t>
+  </si>
+  <si>
+    <t>22131</t>
+  </si>
+  <si>
+    <t>150000.0</t>
+  </si>
+  <si>
+    <t>130000.0</t>
+  </si>
+  <si>
+    <t>120000.0</t>
+  </si>
+  <si>
+    <t>26398</t>
+  </si>
+  <si>
+    <t>22447</t>
+  </si>
+  <si>
+    <t>121499</t>
+  </si>
+  <si>
+    <t>123140</t>
+  </si>
+  <si>
+    <t>142377</t>
+  </si>
+  <si>
+    <t>133942</t>
+  </si>
+  <si>
+    <t>147431</t>
+  </si>
+  <si>
+    <t>221684</t>
+  </si>
+  <si>
+    <t>25003</t>
+  </si>
+  <si>
+    <t>148766</t>
+  </si>
+  <si>
+    <t>120000</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>140000</t>
+  </si>
+  <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>14000</t>
   </si>
 </sst>
 </file>
@@ -407,7 +380,7 @@
         <v>0.041666798293590546</v>
       </c>
       <c r="D10" t="s" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
@@ -421,7 +394,7 @@
         <v>0.03891996294260025</v>
       </c>
       <c r="D11" t="s" s="1">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12">
@@ -435,7 +408,7 @@
         <v>0.030176512897014618</v>
       </c>
       <c r="D12" t="s" s="1">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
@@ -449,7 +422,7 @@
         <v>0.0</v>
       </c>
       <c r="D13" t="s" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
@@ -463,7 +436,7 @@
         <v>0.04304021969437599</v>
       </c>
       <c r="D14" t="s" s="1">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15">
@@ -477,7 +450,7 @@
         <v>0.036753445863723755</v>
       </c>
       <c r="D15" t="s" s="1">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16">
@@ -491,7 +464,7 @@
         <v>0.037043604999780655</v>
       </c>
       <c r="D16" t="s" s="1">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17">
@@ -505,7 +478,7 @@
         <v>0.03781735897064209</v>
       </c>
       <c r="D17" t="s" s="1">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18">
@@ -519,7 +492,7 @@
         <v>0.03859111666679382</v>
       </c>
       <c r="D18" t="s" s="1">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
@@ -533,7 +506,7 @@
         <v>0.04835979640483856</v>
       </c>
       <c r="D19" t="s" s="1">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20">
@@ -547,7 +520,7 @@
         <v>0.0</v>
       </c>
       <c r="D20" t="s" s="1">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21">
@@ -561,7 +534,7 @@
         <v>0.04932698979973793</v>
       </c>
       <c r="D21" t="s" s="1">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22">
@@ -575,7 +548,7 @@
         <v>0.03365841880440712</v>
       </c>
       <c r="D22" t="s" s="1">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23">
@@ -589,7 +562,7 @@
         <v>0.03597968816757202</v>
       </c>
       <c r="D23" t="s" s="1">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24">
@@ -603,7 +576,7 @@
         <v>0.03897799551486969</v>
       </c>
       <c r="D24" t="s" s="1">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25">
@@ -617,7 +590,7 @@
         <v>0.04197630286216736</v>
       </c>
       <c r="D25" t="s" s="1">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26">
@@ -631,7 +604,7 @@
         <v>0.04632868245244026</v>
       </c>
       <c r="D26" t="s" s="1">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27">
@@ -645,7 +618,7 @@
         <v>0.0</v>
       </c>
       <c r="D27" t="s" s="1">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28">
@@ -659,7 +632,7 @@
         <v>0.04468445107340813</v>
       </c>
       <c r="D28" t="s" s="1">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29">
@@ -673,7 +646,7 @@
         <v>0.04004191234707832</v>
       </c>
       <c r="D29" t="s" s="1">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30">
@@ -687,7 +660,7 @@
         <v>0.03665672615170479</v>
       </c>
       <c r="D30" t="s" s="1">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31">
@@ -701,7 +674,7 @@
         <v>0.038030143827199936</v>
       </c>
       <c r="D31" t="s" s="1">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32">
@@ -715,7 +688,7 @@
         <v>0.05116144195199013</v>
       </c>
       <c r="D32" t="s" s="1">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33">
@@ -729,7 +702,7 @@
         <v>0.055130165070295334</v>
       </c>
       <c r="D33" t="s" s="1">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34">
@@ -743,7 +716,7 @@
         <v>0.0</v>
       </c>
       <c r="D34" t="s" s="1">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
class MonthChecker added, which check which month is to be reported. ReportWriter now write only forecasted Turn Over from desired month. added monthly TurnOver
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t/>
   </si>
@@ -123,72 +123,6 @@
   </si>
   <si>
     <t>Pilotaż obrotu</t>
-  </si>
-  <si>
-    <t>25832</t>
-  </si>
-  <si>
-    <t>37363</t>
-  </si>
-  <si>
-    <t>22131</t>
-  </si>
-  <si>
-    <t>150000.0</t>
-  </si>
-  <si>
-    <t>130000.0</t>
-  </si>
-  <si>
-    <t>120000.0</t>
-  </si>
-  <si>
-    <t>26398</t>
-  </si>
-  <si>
-    <t>22447</t>
-  </si>
-  <si>
-    <t>121499</t>
-  </si>
-  <si>
-    <t>123140</t>
-  </si>
-  <si>
-    <t>142377</t>
-  </si>
-  <si>
-    <t>133942</t>
-  </si>
-  <si>
-    <t>147431</t>
-  </si>
-  <si>
-    <t>221684</t>
-  </si>
-  <si>
-    <t>25003</t>
-  </si>
-  <si>
-    <t>148766</t>
-  </si>
-  <si>
-    <t>120000</t>
-  </si>
-  <si>
-    <t>100000</t>
-  </si>
-  <si>
-    <t>140000</t>
-  </si>
-  <si>
-    <t>250000</t>
-  </si>
-  <si>
-    <t>300000</t>
-  </si>
-  <si>
-    <t>14000</t>
   </si>
 </sst>
 </file>
@@ -295,8 +229,8 @@
       <c r="C4" t="n" s="3">
         <v>0.0</v>
       </c>
-      <c r="D4" t="s" s="1">
-        <v>37</v>
+      <c r="D4" t="n" s="1">
+        <v>25832.0</v>
       </c>
     </row>
     <row r="5">
@@ -309,8 +243,8 @@
       <c r="C5" t="n" s="3">
         <v>0.02069799229502678</v>
       </c>
-      <c r="D5" t="s" s="1">
-        <v>38</v>
+      <c r="D5" t="n" s="1">
+        <v>37363.0</v>
       </c>
     </row>
     <row r="6">
@@ -323,8 +257,8 @@
       <c r="C6" t="n" s="3">
         <v>0.0</v>
       </c>
-      <c r="D6" t="s" s="1">
-        <v>39</v>
+      <c r="D6" t="n" s="1">
+        <v>22131.0</v>
       </c>
     </row>
     <row r="7">
@@ -337,8 +271,8 @@
       <c r="C7" t="n" s="3">
         <v>0.040796320885419846</v>
       </c>
-      <c r="D7" t="s" s="1">
-        <v>40</v>
+      <c r="D7" t="n" s="1">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="8">
@@ -351,8 +285,8 @@
       <c r="C8" t="n" s="3">
         <v>0.03433545306324959</v>
       </c>
-      <c r="D8" t="s" s="1">
-        <v>41</v>
+      <c r="D8" t="n" s="1">
+        <v>130000.0</v>
       </c>
     </row>
     <row r="9">
@@ -365,8 +299,8 @@
       <c r="C9" t="n" s="3">
         <v>0.03984847292304039</v>
       </c>
-      <c r="D9" t="s" s="1">
-        <v>42</v>
+      <c r="D9" t="n" s="1">
+        <v>120000.0</v>
       </c>
     </row>
     <row r="10">
@@ -379,8 +313,8 @@
       <c r="C10" t="n" s="3">
         <v>0.041666798293590546</v>
       </c>
-      <c r="D10" t="s" s="1">
-        <v>42</v>
+      <c r="D10" t="n" s="1">
+        <v>120000.0</v>
       </c>
     </row>
     <row r="11">
@@ -393,8 +327,8 @@
       <c r="C11" t="n" s="3">
         <v>0.03891996294260025</v>
       </c>
-      <c r="D11" t="s" s="1">
-        <v>41</v>
+      <c r="D11" t="n" s="1">
+        <v>130000.0</v>
       </c>
     </row>
     <row r="12">
@@ -407,8 +341,8 @@
       <c r="C12" t="n" s="3">
         <v>0.030176512897014618</v>
       </c>
-      <c r="D12" t="s" s="1">
-        <v>40</v>
+      <c r="D12" t="n" s="1">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="13">
@@ -421,8 +355,8 @@
       <c r="C13" t="n" s="3">
         <v>0.0</v>
       </c>
-      <c r="D13" t="s" s="1">
-        <v>43</v>
+      <c r="D13" t="n" s="1">
+        <v>26398.0</v>
       </c>
     </row>
     <row r="14">
@@ -435,8 +369,8 @@
       <c r="C14" t="n" s="3">
         <v>0.04304021969437599</v>
       </c>
-      <c r="D14" t="s" s="1">
-        <v>40</v>
+      <c r="D14" t="n" s="1">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="15">
@@ -449,8 +383,8 @@
       <c r="C15" t="n" s="3">
         <v>0.036753445863723755</v>
       </c>
-      <c r="D15" t="s" s="1">
-        <v>41</v>
+      <c r="D15" t="n" s="1">
+        <v>130000.0</v>
       </c>
     </row>
     <row r="16">
@@ -463,8 +397,8 @@
       <c r="C16" t="n" s="3">
         <v>0.037043604999780655</v>
       </c>
-      <c r="D16" t="s" s="1">
-        <v>42</v>
+      <c r="D16" t="n" s="1">
+        <v>120000.0</v>
       </c>
     </row>
     <row r="17">
@@ -477,8 +411,8 @@
       <c r="C17" t="n" s="3">
         <v>0.03781735897064209</v>
       </c>
-      <c r="D17" t="s" s="1">
-        <v>42</v>
+      <c r="D17" t="n" s="1">
+        <v>120000.0</v>
       </c>
     </row>
     <row r="18">
@@ -491,8 +425,8 @@
       <c r="C18" t="n" s="3">
         <v>0.03859111666679382</v>
       </c>
-      <c r="D18" t="s" s="1">
-        <v>41</v>
+      <c r="D18" t="n" s="1">
+        <v>130000.0</v>
       </c>
     </row>
     <row r="19">
@@ -505,8 +439,8 @@
       <c r="C19" t="n" s="3">
         <v>0.04835979640483856</v>
       </c>
-      <c r="D19" t="s" s="1">
-        <v>40</v>
+      <c r="D19" t="n" s="1">
+        <v>150000.0</v>
       </c>
     </row>
     <row r="20">
@@ -519,8 +453,8 @@
       <c r="C20" t="n" s="3">
         <v>0.0</v>
       </c>
-      <c r="D20" t="s" s="1">
-        <v>44</v>
+      <c r="D20" t="n" s="1">
+        <v>22447.0</v>
       </c>
     </row>
     <row r="21">
@@ -533,8 +467,8 @@
       <c r="C21" t="n" s="3">
         <v>0.04932698979973793</v>
       </c>
-      <c r="D21" t="s" s="1">
-        <v>45</v>
+      <c r="D21" t="n" s="1">
+        <v>121499.0</v>
       </c>
     </row>
     <row r="22">
@@ -547,8 +481,8 @@
       <c r="C22" t="n" s="3">
         <v>0.03365841880440712</v>
       </c>
-      <c r="D22" t="s" s="1">
-        <v>46</v>
+      <c r="D22" t="n" s="1">
+        <v>123140.0</v>
       </c>
     </row>
     <row r="23">
@@ -561,8 +495,8 @@
       <c r="C23" t="n" s="3">
         <v>0.03597968816757202</v>
       </c>
-      <c r="D23" t="s" s="1">
-        <v>47</v>
+      <c r="D23" t="n" s="1">
+        <v>142377.0</v>
       </c>
     </row>
     <row r="24">
@@ -575,8 +509,8 @@
       <c r="C24" t="n" s="3">
         <v>0.03897799551486969</v>
       </c>
-      <c r="D24" t="s" s="1">
-        <v>48</v>
+      <c r="D24" t="n" s="1">
+        <v>133942.0</v>
       </c>
     </row>
     <row r="25">
@@ -589,8 +523,8 @@
       <c r="C25" t="n" s="3">
         <v>0.04197630286216736</v>
       </c>
-      <c r="D25" t="s" s="1">
-        <v>49</v>
+      <c r="D25" t="n" s="1">
+        <v>147431.0</v>
       </c>
     </row>
     <row r="26">
@@ -603,8 +537,8 @@
       <c r="C26" t="n" s="3">
         <v>0.04632868245244026</v>
       </c>
-      <c r="D26" t="s" s="1">
-        <v>50</v>
+      <c r="D26" t="n" s="1">
+        <v>221684.0</v>
       </c>
     </row>
     <row r="27">
@@ -617,8 +551,8 @@
       <c r="C27" t="n" s="3">
         <v>0.0</v>
       </c>
-      <c r="D27" t="s" s="1">
-        <v>51</v>
+      <c r="D27" t="n" s="1">
+        <v>25003.0</v>
       </c>
     </row>
     <row r="28">
@@ -631,8 +565,8 @@
       <c r="C28" t="n" s="3">
         <v>0.04468445107340813</v>
       </c>
-      <c r="D28" t="s" s="1">
-        <v>52</v>
+      <c r="D28" t="n" s="1">
+        <v>148766.0</v>
       </c>
     </row>
     <row r="29">
@@ -645,8 +579,8 @@
       <c r="C29" t="n" s="3">
         <v>0.04004191234707832</v>
       </c>
-      <c r="D29" t="s" s="1">
-        <v>53</v>
+      <c r="D29" t="n" s="1">
+        <v>120000.0</v>
       </c>
     </row>
     <row r="30">
@@ -659,8 +593,8 @@
       <c r="C30" t="n" s="3">
         <v>0.03665672615170479</v>
       </c>
-      <c r="D30" t="s" s="1">
-        <v>54</v>
+      <c r="D30" t="n" s="1">
+        <v>100000.0</v>
       </c>
     </row>
     <row r="31">
@@ -673,8 +607,8 @@
       <c r="C31" t="n" s="3">
         <v>0.038030143827199936</v>
       </c>
-      <c r="D31" t="s" s="1">
-        <v>55</v>
+      <c r="D31" t="n" s="1">
+        <v>140000.0</v>
       </c>
     </row>
     <row r="32">
@@ -687,8 +621,8 @@
       <c r="C32" t="n" s="3">
         <v>0.05116144195199013</v>
       </c>
-      <c r="D32" t="s" s="1">
-        <v>56</v>
+      <c r="D32" t="n" s="1">
+        <v>250000.0</v>
       </c>
     </row>
     <row r="33">
@@ -701,8 +635,8 @@
       <c r="C33" t="n" s="3">
         <v>0.055130165070295334</v>
       </c>
-      <c r="D33" t="s" s="1">
-        <v>57</v>
+      <c r="D33" t="n" s="1">
+        <v>300000.0</v>
       </c>
     </row>
     <row r="34">
@@ -715,8 +649,8 @@
       <c r="C34" t="n" s="3">
         <v>0.0</v>
       </c>
-      <c r="D34" t="s" s="1">
-        <v>58</v>
+      <c r="D34" t="n" s="1">
+        <v>14000.0</v>
       </c>
     </row>
     <row r="35">
@@ -725,6 +659,9 @@
       </c>
       <c r="C35" t="s" s="2">
         <v>35</v>
+      </c>
+      <c r="D35" t="n" s="1">
+        <v>3722013.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
class MonthChecker added, which check which month is to be reported. ReportWriter now write only forecasted Turn Over from desired month. added monthly TurnOver cell formats added
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -129,9 +129,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#.###"/>
     <numFmt numFmtId="165" formatCode="#.##"/>
+    <numFmt numFmtId="166" formatCode="###0,00\ &quot;zł&quot;;-###0,00\ &quot;zł&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -155,7 +156,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -166,17 +167,27 @@
     <border>
       <top style="medium"/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -190,9 +201,9 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="11.3046875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.39453125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.9453125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65234375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.23828125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.98046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -201,16 +212,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="3">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="3">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="3">
         <v>36</v>
       </c>
     </row>
@@ -226,10 +237,10 @@
       <c r="B4" t="n" s="1">
         <v>0.0</v>
       </c>
-      <c r="C4" t="n" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D4" t="n" s="1">
+      <c r="C4" t="n" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n" s="5">
         <v>25832.0</v>
       </c>
     </row>
@@ -240,10 +251,10 @@
       <c r="B5" t="n" s="1">
         <v>107.0</v>
       </c>
-      <c r="C5" t="n" s="3">
+      <c r="C5" t="n" s="4">
         <v>0.02069799229502678</v>
       </c>
-      <c r="D5" t="n" s="1">
+      <c r="D5" t="n" s="5">
         <v>37363.0</v>
       </c>
     </row>
@@ -254,10 +265,10 @@
       <c r="B6" t="n" s="1">
         <v>0.0</v>
       </c>
-      <c r="C6" t="n" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D6" t="n" s="1">
+      <c r="C6" t="n" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D6" t="n" s="5">
         <v>22131.0</v>
       </c>
     </row>
@@ -268,10 +279,10 @@
       <c r="B7" t="n" s="1">
         <v>210.89999389648438</v>
       </c>
-      <c r="C7" t="n" s="3">
+      <c r="C7" t="n" s="4">
         <v>0.040796320885419846</v>
       </c>
-      <c r="D7" t="n" s="1">
+      <c r="D7" t="n" s="5">
         <v>150000.0</v>
       </c>
     </row>
@@ -282,10 +293,10 @@
       <c r="B8" t="n" s="1">
         <v>177.5</v>
       </c>
-      <c r="C8" t="n" s="3">
+      <c r="C8" t="n" s="4">
         <v>0.03433545306324959</v>
       </c>
-      <c r="D8" t="n" s="1">
+      <c r="D8" t="n" s="5">
         <v>130000.0</v>
       </c>
     </row>
@@ -296,10 +307,10 @@
       <c r="B9" t="n" s="1">
         <v>206.0</v>
       </c>
-      <c r="C9" t="n" s="3">
+      <c r="C9" t="n" s="4">
         <v>0.03984847292304039</v>
       </c>
-      <c r="D9" t="n" s="1">
+      <c r="D9" t="n" s="5">
         <v>120000.0</v>
       </c>
     </row>
@@ -310,10 +321,10 @@
       <c r="B10" t="n" s="1">
         <v>215.39999389648438</v>
       </c>
-      <c r="C10" t="n" s="3">
+      <c r="C10" t="n" s="4">
         <v>0.041666798293590546</v>
       </c>
-      <c r="D10" t="n" s="1">
+      <c r="D10" t="n" s="5">
         <v>120000.0</v>
       </c>
     </row>
@@ -324,10 +335,10 @@
       <c r="B11" t="n" s="1">
         <v>201.1999969482422</v>
       </c>
-      <c r="C11" t="n" s="3">
+      <c r="C11" t="n" s="4">
         <v>0.03891996294260025</v>
       </c>
-      <c r="D11" t="n" s="1">
+      <c r="D11" t="n" s="5">
         <v>130000.0</v>
       </c>
     </row>
@@ -338,10 +349,10 @@
       <c r="B12" t="n" s="1">
         <v>156.0</v>
       </c>
-      <c r="C12" t="n" s="3">
+      <c r="C12" t="n" s="4">
         <v>0.030176512897014618</v>
       </c>
-      <c r="D12" t="n" s="1">
+      <c r="D12" t="n" s="5">
         <v>150000.0</v>
       </c>
     </row>
@@ -352,10 +363,10 @@
       <c r="B13" t="n" s="1">
         <v>0.0</v>
       </c>
-      <c r="C13" t="n" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D13" t="n" s="1">
+      <c r="C13" t="n" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n" s="5">
         <v>26398.0</v>
       </c>
     </row>
@@ -366,10 +377,10 @@
       <c r="B14" t="n" s="1">
         <v>222.5</v>
       </c>
-      <c r="C14" t="n" s="3">
+      <c r="C14" t="n" s="4">
         <v>0.04304021969437599</v>
       </c>
-      <c r="D14" t="n" s="1">
+      <c r="D14" t="n" s="5">
         <v>150000.0</v>
       </c>
     </row>
@@ -380,10 +391,10 @@
       <c r="B15" t="n" s="1">
         <v>190.0</v>
       </c>
-      <c r="C15" t="n" s="3">
+      <c r="C15" t="n" s="4">
         <v>0.036753445863723755</v>
       </c>
-      <c r="D15" t="n" s="1">
+      <c r="D15" t="n" s="5">
         <v>130000.0</v>
       </c>
     </row>
@@ -394,10 +405,10 @@
       <c r="B16" t="n" s="1">
         <v>191.5</v>
       </c>
-      <c r="C16" t="n" s="3">
+      <c r="C16" t="n" s="4">
         <v>0.037043604999780655</v>
       </c>
-      <c r="D16" t="n" s="1">
+      <c r="D16" t="n" s="5">
         <v>120000.0</v>
       </c>
     </row>
@@ -408,10 +419,10 @@
       <c r="B17" t="n" s="1">
         <v>195.5</v>
       </c>
-      <c r="C17" t="n" s="3">
+      <c r="C17" t="n" s="4">
         <v>0.03781735897064209</v>
       </c>
-      <c r="D17" t="n" s="1">
+      <c r="D17" t="n" s="5">
         <v>120000.0</v>
       </c>
     </row>
@@ -422,10 +433,10 @@
       <c r="B18" t="n" s="1">
         <v>199.5</v>
       </c>
-      <c r="C18" t="n" s="3">
+      <c r="C18" t="n" s="4">
         <v>0.03859111666679382</v>
       </c>
-      <c r="D18" t="n" s="1">
+      <c r="D18" t="n" s="5">
         <v>130000.0</v>
       </c>
     </row>
@@ -436,10 +447,10 @@
       <c r="B19" t="n" s="1">
         <v>250.0</v>
       </c>
-      <c r="C19" t="n" s="3">
+      <c r="C19" t="n" s="4">
         <v>0.04835979640483856</v>
       </c>
-      <c r="D19" t="n" s="1">
+      <c r="D19" t="n" s="5">
         <v>150000.0</v>
       </c>
     </row>
@@ -450,10 +461,10 @@
       <c r="B20" t="n" s="1">
         <v>0.0</v>
       </c>
-      <c r="C20" t="n" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D20" t="n" s="1">
+      <c r="C20" t="n" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D20" t="n" s="5">
         <v>22447.0</v>
       </c>
     </row>
@@ -464,10 +475,10 @@
       <c r="B21" t="n" s="1">
         <v>255.0</v>
       </c>
-      <c r="C21" t="n" s="3">
+      <c r="C21" t="n" s="4">
         <v>0.04932698979973793</v>
       </c>
-      <c r="D21" t="n" s="1">
+      <c r="D21" t="n" s="5">
         <v>121499.0</v>
       </c>
     </row>
@@ -478,10 +489,10 @@
       <c r="B22" t="n" s="1">
         <v>174.0</v>
       </c>
-      <c r="C22" t="n" s="3">
+      <c r="C22" t="n" s="4">
         <v>0.03365841880440712</v>
       </c>
-      <c r="D22" t="n" s="1">
+      <c r="D22" t="n" s="5">
         <v>123140.0</v>
       </c>
     </row>
@@ -492,10 +503,10 @@
       <c r="B23" t="n" s="1">
         <v>186.0</v>
       </c>
-      <c r="C23" t="n" s="3">
+      <c r="C23" t="n" s="4">
         <v>0.03597968816757202</v>
       </c>
-      <c r="D23" t="n" s="1">
+      <c r="D23" t="n" s="5">
         <v>142377.0</v>
       </c>
     </row>
@@ -506,10 +517,10 @@
       <c r="B24" t="n" s="1">
         <v>201.5</v>
       </c>
-      <c r="C24" t="n" s="3">
+      <c r="C24" t="n" s="4">
         <v>0.03897799551486969</v>
       </c>
-      <c r="D24" t="n" s="1">
+      <c r="D24" t="n" s="5">
         <v>133942.0</v>
       </c>
     </row>
@@ -520,10 +531,10 @@
       <c r="B25" t="n" s="1">
         <v>217.0</v>
       </c>
-      <c r="C25" t="n" s="3">
+      <c r="C25" t="n" s="4">
         <v>0.04197630286216736</v>
       </c>
-      <c r="D25" t="n" s="1">
+      <c r="D25" t="n" s="5">
         <v>147431.0</v>
       </c>
     </row>
@@ -534,10 +545,10 @@
       <c r="B26" t="n" s="1">
         <v>239.5</v>
       </c>
-      <c r="C26" t="n" s="3">
+      <c r="C26" t="n" s="4">
         <v>0.04632868245244026</v>
       </c>
-      <c r="D26" t="n" s="1">
+      <c r="D26" t="n" s="5">
         <v>221684.0</v>
       </c>
     </row>
@@ -548,10 +559,10 @@
       <c r="B27" t="n" s="1">
         <v>0.0</v>
       </c>
-      <c r="C27" t="n" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D27" t="n" s="1">
+      <c r="C27" t="n" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D27" t="n" s="5">
         <v>25003.0</v>
       </c>
     </row>
@@ -562,10 +573,10 @@
       <c r="B28" t="n" s="1">
         <v>231.0</v>
       </c>
-      <c r="C28" t="n" s="3">
+      <c r="C28" t="n" s="4">
         <v>0.04468445107340813</v>
       </c>
-      <c r="D28" t="n" s="1">
+      <c r="D28" t="n" s="5">
         <v>148766.0</v>
       </c>
     </row>
@@ -576,10 +587,10 @@
       <c r="B29" t="n" s="1">
         <v>207.0</v>
       </c>
-      <c r="C29" t="n" s="3">
+      <c r="C29" t="n" s="4">
         <v>0.04004191234707832</v>
       </c>
-      <c r="D29" t="n" s="1">
+      <c r="D29" t="n" s="5">
         <v>120000.0</v>
       </c>
     </row>
@@ -590,10 +601,10 @@
       <c r="B30" t="n" s="1">
         <v>189.5</v>
       </c>
-      <c r="C30" t="n" s="3">
+      <c r="C30" t="n" s="4">
         <v>0.03665672615170479</v>
       </c>
-      <c r="D30" t="n" s="1">
+      <c r="D30" t="n" s="5">
         <v>100000.0</v>
       </c>
     </row>
@@ -604,10 +615,10 @@
       <c r="B31" t="n" s="1">
         <v>196.60000610351562</v>
       </c>
-      <c r="C31" t="n" s="3">
+      <c r="C31" t="n" s="4">
         <v>0.038030143827199936</v>
       </c>
-      <c r="D31" t="n" s="1">
+      <c r="D31" t="n" s="5">
         <v>140000.0</v>
       </c>
     </row>
@@ -618,10 +629,10 @@
       <c r="B32" t="n" s="1">
         <v>264.48333740234375</v>
       </c>
-      <c r="C32" t="n" s="3">
+      <c r="C32" t="n" s="4">
         <v>0.05116144195199013</v>
       </c>
-      <c r="D32" t="n" s="1">
+      <c r="D32" t="n" s="5">
         <v>250000.0</v>
       </c>
     </row>
@@ -632,10 +643,10 @@
       <c r="B33" t="n" s="1">
         <v>285.0</v>
       </c>
-      <c r="C33" t="n" s="3">
+      <c r="C33" t="n" s="4">
         <v>0.055130165070295334</v>
       </c>
-      <c r="D33" t="n" s="1">
+      <c r="D33" t="n" s="5">
         <v>300000.0</v>
       </c>
     </row>
@@ -646,10 +657,10 @@
       <c r="B34" t="n" s="1">
         <v>0.0</v>
       </c>
-      <c r="C34" t="n" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D34" t="n" s="1">
+      <c r="C34" t="n" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D34" t="n" s="5">
         <v>14000.0</v>
       </c>
     </row>
@@ -660,7 +671,7 @@
       <c r="C35" t="s" s="2">
         <v>35</v>
       </c>
-      <c r="D35" t="n" s="1">
+      <c r="D35" t="n" s="6">
         <v>3722013.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
class MonthChecker added, which check which month is to be reported. ReportWriter now write only forecasted Turn Over from desired month. added monthly TurnOver cell formats added method to calc and write daily share in monthly turn over added.
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t/>
   </si>
@@ -116,13 +116,16 @@
     <t>Suma godzin</t>
   </si>
   <si>
-    <t>Udział dnia</t>
+    <t>Udział dnia w godzinach</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
     <t>Pilotaż obrotu</t>
+  </si>
+  <si>
+    <t>Udział dnia w TO</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -202,8 +205,9 @@
   <cols>
     <col min="1" max="1" width="11.3046875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.65234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.23828125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="23.0625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.98046875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="16.44921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -224,6 +228,9 @@
       <c r="D2" t="s" s="3">
         <v>36</v>
       </c>
+      <c r="E2" t="s" s="3">
+        <v>37</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -243,6 +250,9 @@
       <c r="D4" t="n" s="5">
         <v>25832.0</v>
       </c>
+      <c r="E4" t="n" s="4">
+        <v>0.006940330407228561</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -257,6 +267,9 @@
       <c r="D5" t="n" s="5">
         <v>37363.0</v>
       </c>
+      <c r="E5" t="n" s="4">
+        <v>0.010038385142663392</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -271,6 +284,9 @@
       <c r="D6" t="n" s="5">
         <v>22131.0</v>
       </c>
+      <c r="E6" t="n" s="4">
+        <v>0.00594597600814398</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -285,6 +301,9 @@
       <c r="D7" t="n" s="5">
         <v>150000.0</v>
       </c>
+      <c r="E7" t="n" s="4">
+        <v>0.040300772727016265</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -299,6 +318,9 @@
       <c r="D8" t="n" s="5">
         <v>130000.0</v>
       </c>
+      <c r="E8" t="n" s="4">
+        <v>0.0349273363634141</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -313,6 +335,9 @@
       <c r="D9" t="n" s="5">
         <v>120000.0</v>
       </c>
+      <c r="E9" t="n" s="4">
+        <v>0.032240618181613015</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -327,6 +352,9 @@
       <c r="D10" t="n" s="5">
         <v>120000.0</v>
       </c>
+      <c r="E10" t="n" s="4">
+        <v>0.032240618181613015</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -341,6 +369,9 @@
       <c r="D11" t="n" s="5">
         <v>130000.0</v>
       </c>
+      <c r="E11" t="n" s="4">
+        <v>0.0349273363634141</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -355,6 +386,9 @@
       <c r="D12" t="n" s="5">
         <v>150000.0</v>
       </c>
+      <c r="E12" t="n" s="4">
+        <v>0.040300772727016265</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -369,6 +403,9 @@
       <c r="D13" t="n" s="5">
         <v>26398.0</v>
       </c>
+      <c r="E13" t="n" s="4">
+        <v>0.007092398656318503</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -383,6 +420,9 @@
       <c r="D14" t="n" s="5">
         <v>150000.0</v>
       </c>
+      <c r="E14" t="n" s="4">
+        <v>0.040300772727016265</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -397,6 +437,9 @@
       <c r="D15" t="n" s="5">
         <v>130000.0</v>
       </c>
+      <c r="E15" t="n" s="4">
+        <v>0.0349273363634141</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -411,6 +454,9 @@
       <c r="D16" t="n" s="5">
         <v>120000.0</v>
       </c>
+      <c r="E16" t="n" s="4">
+        <v>0.032240618181613015</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -425,6 +471,9 @@
       <c r="D17" t="n" s="5">
         <v>120000.0</v>
       </c>
+      <c r="E17" t="n" s="4">
+        <v>0.032240618181613015</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -439,6 +488,9 @@
       <c r="D18" t="n" s="5">
         <v>130000.0</v>
       </c>
+      <c r="E18" t="n" s="4">
+        <v>0.0349273363634141</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -453,6 +505,9 @@
       <c r="D19" t="n" s="5">
         <v>150000.0</v>
       </c>
+      <c r="E19" t="n" s="4">
+        <v>0.040300772727016265</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -467,6 +522,9 @@
       <c r="D20" t="n" s="5">
         <v>22447.0</v>
       </c>
+      <c r="E20" t="n" s="4">
+        <v>0.006030876302688894</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -481,6 +539,9 @@
       <c r="D21" t="n" s="5">
         <v>121499.0</v>
       </c>
+      <c r="E21" t="n" s="4">
+        <v>0.032643357237065</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -495,6 +556,9 @@
       <c r="D22" t="n" s="5">
         <v>123140.0</v>
       </c>
+      <c r="E22" t="n" s="4">
+        <v>0.03308424769069856</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -509,6 +573,9 @@
       <c r="D23" t="n" s="5">
         <v>142377.0</v>
       </c>
+      <c r="E23" t="n" s="4">
+        <v>0.038252687457029304</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -523,6 +590,9 @@
       <c r="D24" t="n" s="5">
         <v>133942.0</v>
       </c>
+      <c r="E24" t="n" s="4">
+        <v>0.03598644067068009</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -537,6 +607,9 @@
       <c r="D25" t="n" s="5">
         <v>147431.0</v>
       </c>
+      <c r="E25" t="n" s="4">
+        <v>0.03961055482611157</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -551,6 +624,9 @@
       <c r="D26" t="n" s="5">
         <v>221684.0</v>
       </c>
+      <c r="E26" t="n" s="4">
+        <v>0.05956024334143916</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -565,6 +641,9 @@
       <c r="D27" t="n" s="5">
         <v>25003.0</v>
       </c>
+      <c r="E27" t="n" s="4">
+        <v>0.006717601469957251</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -579,6 +658,9 @@
       <c r="D28" t="n" s="5">
         <v>148766.0</v>
       </c>
+      <c r="E28" t="n" s="4">
+        <v>0.03996923170338201</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
@@ -593,6 +675,9 @@
       <c r="D29" t="n" s="5">
         <v>120000.0</v>
       </c>
+      <c r="E29" t="n" s="4">
+        <v>0.032240618181613015</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -607,6 +692,9 @@
       <c r="D30" t="n" s="5">
         <v>100000.0</v>
       </c>
+      <c r="E30" t="n" s="4">
+        <v>0.026867181818010843</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
@@ -621,6 +709,9 @@
       <c r="D31" t="n" s="5">
         <v>140000.0</v>
       </c>
+      <c r="E31" t="n" s="4">
+        <v>0.037614054545215186</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -635,6 +726,9 @@
       <c r="D32" t="n" s="5">
         <v>250000.0</v>
       </c>
+      <c r="E32" t="n" s="4">
+        <v>0.06716795454502711</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -649,6 +743,9 @@
       <c r="D33" t="n" s="5">
         <v>300000.0</v>
       </c>
+      <c r="E33" t="n" s="4">
+        <v>0.08060154545403253</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
@@ -663,6 +760,9 @@
       <c r="D34" t="n" s="5">
         <v>14000.0</v>
       </c>
+      <c r="E34" t="n" s="4">
+        <v>0.0037614054545215183</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" t="n" s="2">
@@ -673,6 +773,9 @@
       </c>
       <c r="D35" t="n" s="6">
         <v>3722013.0</v>
+      </c>
+      <c r="E35" t="n" s="2">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PerfectHours column added, considering close days
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -248,7 +248,7 @@
         <v>0.044477378631061694</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>355.744660380989</v>
+        <v>358.61964128073913</v>
       </c>
     </row>
     <row r="5">
@@ -268,7 +268,7 @@
         <v>0.036461389924843345</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>118.58155346032966</v>
+        <v>119.53988042691306</v>
       </c>
     </row>
     <row r="6">
@@ -288,7 +288,7 @@
         <v>0.026530650879892693</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>118.58155346032966</v>
+        <v>119.53988042691306</v>
       </c>
     </row>
     <row r="7">
@@ -308,7 +308,7 @@
         <v>0.03532552107983265</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>118.58155346032966</v>
+        <v>119.53988042691306</v>
       </c>
     </row>
     <row r="8">
@@ -328,7 +328,7 @@
         <v>0.04360113695062487</v>
       </c>
       <c r="F8" t="n" s="2">
-        <v>118.58155346032966</v>
+        <v>119.53988042691306</v>
       </c>
     </row>
     <row r="9">
@@ -348,7 +348,7 @@
         <v>0.04541852710264198</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>272.7375729587582</v>
+        <v>274.9417249819</v>
       </c>
     </row>
     <row r="10">
@@ -368,7 +368,7 @@
         <v>0.0</v>
       </c>
       <c r="F10" t="n" s="2">
-        <v>8.300708742223076</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -388,7 +388,7 @@
         <v>0.039998810042162374</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>207.51771855557692</v>
+        <v>209.19479074709787</v>
       </c>
     </row>
     <row r="12">
@@ -408,7 +408,7 @@
         <v>0.03651007001820095</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>201.5886408825604</v>
+        <v>203.21779672575215</v>
       </c>
     </row>
     <row r="13">
@@ -428,7 +428,7 @@
         <v>0.03706177774292043</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>284.5957283047912</v>
+        <v>286.89571302459126</v>
       </c>
     </row>
     <row r="14">
@@ -448,7 +448,7 @@
         <v>0.0</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>8.300708742223076</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
@@ -468,7 +468,7 @@
         <v>0.04571060766278759</v>
       </c>
       <c r="F15" t="n" s="2">
-        <v>320.1701943428901</v>
+        <v>322.7576771526652</v>
       </c>
     </row>
     <row r="16">
@@ -488,7 +488,7 @@
         <v>0.04368497488918524</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>355.744660380989</v>
+        <v>358.61964128073913</v>
       </c>
     </row>
     <row r="17">
@@ -508,7 +508,7 @@
         <v>0.0</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>16.601417484446152</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -528,7 +528,7 @@
         <v>0.04773894488602098</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>237.16310692065932</v>
+        <v>239.07976085382612</v>
       </c>
     </row>
     <row r="19">
@@ -548,7 +548,7 @@
         <v>0.03133645787414038</v>
       </c>
       <c r="F19" t="n" s="2">
-        <v>189.73048553652745</v>
+        <v>191.2638086830609</v>
       </c>
     </row>
     <row r="20">
@@ -568,7 +568,7 @@
         <v>0.027909920191691393</v>
       </c>
       <c r="F20" t="n" s="2">
-        <v>177.8723301904945</v>
+        <v>179.30982064036957</v>
       </c>
     </row>
     <row r="21">
@@ -588,7 +588,7 @@
         <v>0.032255970748672744</v>
       </c>
       <c r="F21" t="n" s="2">
-        <v>177.8723301904945</v>
+        <v>179.30982064036957</v>
       </c>
     </row>
     <row r="22">
@@ -608,7 +608,7 @@
         <v>0.04274112196797391</v>
       </c>
       <c r="F22" t="n" s="2">
-        <v>237.16310692065932</v>
+        <v>239.07976085382612</v>
       </c>
     </row>
     <row r="23">
@@ -628,7 +628,7 @@
         <v>0.038911621290509284</v>
       </c>
       <c r="F23" t="n" s="2">
-        <v>355.744660380989</v>
+        <v>358.61964128073913</v>
       </c>
     </row>
     <row r="24">
@@ -648,7 +648,7 @@
         <v>0.0</v>
       </c>
       <c r="F24" t="n" s="2">
-        <v>16.601417484446152</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25">
@@ -668,7 +668,7 @@
         <v>0.04515078658917518</v>
       </c>
       <c r="F25" t="n" s="2">
-        <v>237.16310692065932</v>
+        <v>239.07976085382612</v>
       </c>
     </row>
     <row r="26">
@@ -688,7 +688,7 @@
         <v>0.035942135595695604</v>
       </c>
       <c r="F26" t="n" s="2">
-        <v>189.73048553652745</v>
+        <v>191.2638086830609</v>
       </c>
     </row>
     <row r="27">
@@ -708,7 +708,7 @@
         <v>0.030668458815288797</v>
       </c>
       <c r="F27" t="n" s="2">
-        <v>177.8723301904945</v>
+        <v>179.30982064036957</v>
       </c>
     </row>
     <row r="28">
@@ -728,7 +728,7 @@
         <v>0.03274547613187979</v>
       </c>
       <c r="F28" t="n" s="2">
-        <v>201.5886408825604</v>
+        <v>203.21779672575215</v>
       </c>
     </row>
     <row r="29">
@@ -748,7 +748,7 @@
         <v>0.04194601377646642</v>
       </c>
       <c r="F29" t="n" s="2">
-        <v>296.45388365082414</v>
+        <v>298.84970106728264</v>
       </c>
     </row>
     <row r="30">
@@ -768,7 +768,7 @@
         <v>0.04460719221334863</v>
       </c>
       <c r="F30" t="n" s="2">
-        <v>355.744660380989</v>
+        <v>358.61964128073913</v>
       </c>
     </row>
     <row r="31">
@@ -788,7 +788,7 @@
         <v>0.03562301053924016</v>
       </c>
       <c r="F31" t="n" s="2">
-        <v>320.1701943428901</v>
+        <v>322.7576771526652</v>
       </c>
     </row>
     <row r="32">
@@ -808,7 +808,7 @@
         <v>0.04066140020175189</v>
       </c>
       <c r="F32" t="n" s="2">
-        <v>249.0212622666923</v>
+        <v>251.0337488965174</v>
       </c>
     </row>
     <row r="33">
@@ -828,7 +828,7 @@
         <v>0.0369806442539911</v>
       </c>
       <c r="F33" t="n" s="2">
-        <v>237.16310692065932</v>
+        <v>239.07976085382612</v>
       </c>
     </row>
     <row r="34">
@@ -848,7 +848,7 @@
         <v>1.0</v>
       </c>
       <c r="F34" t="n" s="3">
-        <v>6162.6833333333325</v>
+        <v>6162.280836007368</v>
       </c>
     </row>
     <row r="35"/>

</xml_diff>

<commit_message>
Difference in hours column added, considering close days
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Dzień</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>"Idealne" godziny</t>
+  </si>
+  <si>
+    <t>Różnica godzin</t>
   </si>
 </sst>
 </file>
@@ -130,8 +133,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="#.###"/>
-    <numFmt numFmtId="165" formatCode="#.##"/>
+    <numFmt numFmtId="164" formatCode="#.#"/>
+    <numFmt numFmtId="165" formatCode="#"/>
     <numFmt numFmtId="166" formatCode="###0,00\ &quot;zł&quot;;-###0,00\ &quot;zł&quot;"/>
   </numFmts>
   <fonts count="2">
@@ -195,7 +198,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -207,6 +210,7 @@
     <col min="2" max="2" width="13.98046875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1"/>
@@ -229,6 +233,9 @@
       <c r="F2" t="s" s="4">
         <v>36</v>
       </c>
+      <c r="G2" t="s" s="4">
+        <v>37</v>
+      </c>
     </row>
     <row r="3"/>
     <row r="4">
@@ -250,6 +257,9 @@
       <c r="F4" t="n" s="2">
         <v>358.61964128073913</v>
       </c>
+      <c r="G4" t="n" s="2">
+        <v>-84.51964128073911</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="1">
@@ -270,6 +280,9 @@
       <c r="F5" t="n" s="2">
         <v>119.53988042691306</v>
       </c>
+      <c r="G5" t="n" s="2">
+        <v>105.16011957308693</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="1">
@@ -290,6 +303,9 @@
       <c r="F6" t="n" s="2">
         <v>119.53988042691306</v>
       </c>
+      <c r="G6" t="n" s="2">
+        <v>43.96011957308694</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="1">
@@ -310,6 +326,9 @@
       <c r="F7" t="n" s="2">
         <v>119.53988042691306</v>
       </c>
+      <c r="G7" t="n" s="2">
+        <v>98.16011957308693</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="1">
@@ -330,6 +349,9 @@
       <c r="F8" t="n" s="2">
         <v>119.53988042691306</v>
       </c>
+      <c r="G8" t="n" s="2">
+        <v>149.16011957308694</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="1">
@@ -350,6 +372,9 @@
       <c r="F9" t="n" s="2">
         <v>274.9417249819</v>
       </c>
+      <c r="G9" t="n" s="2">
+        <v>4.958275018099982</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="1">
@@ -370,6 +395,9 @@
       <c r="F10" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="G10" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="1">
@@ -390,6 +418,9 @@
       <c r="F11" t="n" s="2">
         <v>209.19479074709787</v>
       </c>
+      <c r="G11" t="n" s="2">
+        <v>37.30520925290213</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="1">
@@ -410,6 +441,9 @@
       <c r="F12" t="n" s="2">
         <v>203.21779672575215</v>
       </c>
+      <c r="G12" t="n" s="2">
+        <v>21.78220327424785</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="1">
@@ -430,6 +464,9 @@
       <c r="F13" t="n" s="2">
         <v>286.89571302459126</v>
       </c>
+      <c r="G13" t="n" s="2">
+        <v>-58.495713024591254</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="1">
@@ -450,6 +487,9 @@
       <c r="F14" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="G14" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="1">
@@ -470,6 +510,9 @@
       <c r="F15" t="n" s="2">
         <v>322.7576771526652</v>
       </c>
+      <c r="G15" t="n" s="2">
+        <v>-41.057677152665235</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="1">
@@ -490,6 +533,9 @@
       <c r="F16" t="n" s="2">
         <v>358.61964128073913</v>
       </c>
+      <c r="G16" t="n" s="2">
+        <v>-89.4029746140721</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="1">
@@ -510,6 +556,9 @@
       <c r="F17" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="G17" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="1">
@@ -530,6 +579,9 @@
       <c r="F18" t="n" s="2">
         <v>239.07976085382612</v>
       </c>
+      <c r="G18" t="n" s="2">
+        <v>55.12023914617387</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="1">
@@ -550,6 +602,9 @@
       <c r="F19" t="n" s="2">
         <v>191.2638086830609</v>
       </c>
+      <c r="G19" t="n" s="2">
+        <v>1.8528579836061283</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="1">
@@ -570,6 +625,9 @@
       <c r="F20" t="n" s="2">
         <v>179.30982064036957</v>
       </c>
+      <c r="G20" t="n" s="2">
+        <v>-7.309820640369566</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="1">
@@ -590,6 +648,9 @@
       <c r="F21" t="n" s="2">
         <v>179.30982064036957</v>
       </c>
+      <c r="G21" t="n" s="2">
+        <v>19.473512692963453</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="1">
@@ -610,6 +671,9 @@
       <c r="F22" t="n" s="2">
         <v>239.07976085382612</v>
       </c>
+      <c r="G22" t="n" s="2">
+        <v>24.32023914617386</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="1">
@@ -630,6 +694,9 @@
       <c r="F23" t="n" s="2">
         <v>358.61964128073913</v>
       </c>
+      <c r="G23" t="n" s="2">
+        <v>-118.81964128073912</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="1">
@@ -650,6 +717,9 @@
       <c r="F24" t="n" s="2">
         <v>0.0</v>
       </c>
+      <c r="G24" t="n" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="1">
@@ -670,6 +740,9 @@
       <c r="F25" t="n" s="2">
         <v>239.07976085382612</v>
       </c>
+      <c r="G25" t="n" s="2">
+        <v>39.170239146173884</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="1">
@@ -690,6 +763,9 @@
       <c r="F26" t="n" s="2">
         <v>191.2638086830609</v>
       </c>
+      <c r="G26" t="n" s="2">
+        <v>30.236191316939113</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="1">
@@ -710,6 +786,9 @@
       <c r="F27" t="n" s="2">
         <v>179.30982064036957</v>
       </c>
+      <c r="G27" t="n" s="2">
+        <v>9.690179359630434</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="1">
@@ -730,6 +809,9 @@
       <c r="F28" t="n" s="2">
         <v>203.21779672575215</v>
       </c>
+      <c r="G28" t="n" s="2">
+        <v>-1.4177967257521402</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="1">
@@ -750,6 +832,9 @@
       <c r="F29" t="n" s="2">
         <v>298.84970106728264</v>
       </c>
+      <c r="G29" t="n" s="2">
+        <v>-40.34970106728264</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="1">
@@ -770,6 +855,9 @@
       <c r="F30" t="n" s="2">
         <v>358.61964128073913</v>
       </c>
+      <c r="G30" t="n" s="2">
+        <v>-83.71964128073915</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="1">
@@ -790,6 +878,9 @@
       <c r="F31" t="n" s="2">
         <v>322.7576771526652</v>
       </c>
+      <c r="G31" t="n" s="2">
+        <v>-103.22434381933223</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="1">
@@ -810,6 +901,9 @@
       <c r="F32" t="n" s="2">
         <v>251.0337488965174</v>
       </c>
+      <c r="G32" t="n" s="2">
+        <v>-0.4504155631844071</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="1">
@@ -830,6 +924,9 @@
       <c r="F33" t="n" s="2">
         <v>239.07976085382612</v>
       </c>
+      <c r="G33" t="n" s="2">
+        <v>-11.17976085382611</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="3">
@@ -849,6 +946,9 @@
       </c>
       <c r="F34" t="n" s="3">
         <v>6162.280836007368</v>
+      </c>
+      <c r="G34" t="n" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="35"/>

</xml_diff>

<commit_message>
added method to map department name and monthly forecast in ForecastReader
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -243,10 +243,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="n" s="6">
-        <v>300000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="C4" t="n" s="5">
-        <v>0.05772561092938234</v>
+        <v>0.02326934264107039</v>
       </c>
       <c r="D4" t="n" s="2">
         <v>274.1</v>
@@ -255,10 +255,10 @@
         <v>0.044477378631061694</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>358.61964128073913</v>
+        <v>144.56949132887596</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>-84.51964128073911</v>
+        <v>129.53050867112407</v>
       </c>
     </row>
     <row r="5">
@@ -266,10 +266,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="n" s="6">
-        <v>100000.0</v>
+        <v>200000.0</v>
       </c>
       <c r="C5" t="n" s="5">
-        <v>0.01924187030979411</v>
+        <v>0.03878223773511732</v>
       </c>
       <c r="D5" t="n" s="2">
         <v>224.7</v>
@@ -278,10 +278,10 @@
         <v>0.036461389924843345</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>119.53988042691306</v>
+        <v>240.94915221479326</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>105.16011957308693</v>
+        <v>-16.24915221479327</v>
       </c>
     </row>
     <row r="6">
@@ -289,10 +289,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="n" s="6">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="C6" t="n" s="5">
-        <v>0.01924187030979411</v>
+        <v>0.02326934264107039</v>
       </c>
       <c r="D6" t="n" s="2">
         <v>163.5</v>
@@ -301,10 +301,10 @@
         <v>0.026530650879892693</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>119.53988042691306</v>
+        <v>144.56949132887596</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>43.96011957308694</v>
+        <v>18.930508671124045</v>
       </c>
     </row>
     <row r="7">
@@ -312,10 +312,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="n" s="6">
-        <v>100000.0</v>
+        <v>120000.0</v>
       </c>
       <c r="C7" t="n" s="5">
-        <v>0.01924187030979411</v>
+        <v>0.02326934264107039</v>
       </c>
       <c r="D7" t="n" s="2">
         <v>217.7</v>
@@ -324,10 +324,10 @@
         <v>0.03532552107983265</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>119.53988042691306</v>
+        <v>144.56949132887596</v>
       </c>
       <c r="G7" t="n" s="2">
-        <v>98.16011957308693</v>
+        <v>73.13050867112403</v>
       </c>
     </row>
     <row r="8">
@@ -338,7 +338,7 @@
         <v>100000.0</v>
       </c>
       <c r="C8" t="n" s="5">
-        <v>0.01924187030979411</v>
+        <v>0.01939111886755866</v>
       </c>
       <c r="D8" t="n" s="2">
         <v>268.7</v>
@@ -347,10 +347,10 @@
         <v>0.04360113695062487</v>
       </c>
       <c r="F8" t="n" s="2">
-        <v>119.53988042691306</v>
+        <v>120.47457610739663</v>
       </c>
       <c r="G8" t="n" s="2">
-        <v>149.16011957308694</v>
+        <v>148.22542389260337</v>
       </c>
     </row>
     <row r="9">
@@ -361,7 +361,7 @@
         <v>230000.0</v>
       </c>
       <c r="C9" t="n" s="5">
-        <v>0.04425630171252646</v>
+        <v>0.044599573395384916</v>
       </c>
       <c r="D9" t="n" s="2">
         <v>279.9</v>
@@ -370,10 +370,10 @@
         <v>0.04541852710264198</v>
       </c>
       <c r="F9" t="n" s="2">
-        <v>274.9417249819</v>
+        <v>277.0915250470123</v>
       </c>
       <c r="G9" t="n" s="2">
-        <v>4.958275018099982</v>
+        <v>2.8084749529876945</v>
       </c>
     </row>
     <row r="10">
@@ -384,7 +384,7 @@
         <v>7000.0</v>
       </c>
       <c r="C10" t="n" s="5">
-        <v>0.0013469309216855877</v>
+        <v>0.001357378320729106</v>
       </c>
       <c r="D10" t="n" s="2">
         <v>0.0</v>
@@ -407,7 +407,7 @@
         <v>175000.0</v>
       </c>
       <c r="C11" t="n" s="5">
-        <v>0.0336732730421397</v>
+        <v>0.03393445801822765</v>
       </c>
       <c r="D11" t="n" s="2">
         <v>246.5</v>
@@ -416,10 +416,10 @@
         <v>0.039998810042162374</v>
       </c>
       <c r="F11" t="n" s="2">
-        <v>209.19479074709787</v>
+        <v>210.83050818794408</v>
       </c>
       <c r="G11" t="n" s="2">
-        <v>37.30520925290213</v>
+        <v>35.669491812055924</v>
       </c>
     </row>
     <row r="12">
@@ -430,7 +430,7 @@
         <v>170000.0</v>
       </c>
       <c r="C12" t="n" s="5">
-        <v>0.03271117952664999</v>
+        <v>0.03296490207484972</v>
       </c>
       <c r="D12" t="n" s="2">
         <v>225.0</v>
@@ -439,10 +439,10 @@
         <v>0.03651007001820095</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>203.21779672575215</v>
+        <v>204.8067793825743</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>21.78220327424785</v>
+        <v>20.19322061742571</v>
       </c>
     </row>
     <row r="13">
@@ -453,7 +453,7 @@
         <v>240000.0</v>
       </c>
       <c r="C13" t="n" s="5">
-        <v>0.04618048874350587</v>
+        <v>0.04653868528214078</v>
       </c>
       <c r="D13" t="n" s="2">
         <v>228.4</v>
@@ -462,10 +462,10 @@
         <v>0.03706177774292043</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>286.89571302459126</v>
+        <v>289.1389826577519</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>-58.495713024591254</v>
+        <v>-60.738982657751905</v>
       </c>
     </row>
     <row r="14">
@@ -476,7 +476,7 @@
         <v>7000.0</v>
       </c>
       <c r="C14" t="n" s="5">
-        <v>0.0013469309216855877</v>
+        <v>0.001357378320729106</v>
       </c>
       <c r="D14" t="n" s="2">
         <v>0.0</v>
@@ -499,7 +499,7 @@
         <v>270000.0</v>
       </c>
       <c r="C15" t="n" s="5">
-        <v>0.0519530498364441</v>
+        <v>0.05235602094240838</v>
       </c>
       <c r="D15" t="n" s="2">
         <v>281.7</v>
@@ -508,10 +508,10 @@
         <v>0.04571060766278759</v>
       </c>
       <c r="F15" t="n" s="2">
-        <v>322.7576771526652</v>
+        <v>325.2813554899709</v>
       </c>
       <c r="G15" t="n" s="2">
-        <v>-41.057677152665235</v>
+        <v>-43.58135548997092</v>
       </c>
     </row>
     <row r="16">
@@ -522,7 +522,7 @@
         <v>300000.0</v>
       </c>
       <c r="C16" t="n" s="5">
-        <v>0.05772561092938234</v>
+        <v>0.058173356602675974</v>
       </c>
       <c r="D16" t="n" s="2">
         <v>269.21666666666704</v>
@@ -531,10 +531,10 @@
         <v>0.04368497488918524</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>358.61964128073913</v>
+        <v>361.4237283221899</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>-89.4029746140721</v>
+        <v>-92.20706165552286</v>
       </c>
     </row>
     <row r="17">
@@ -545,7 +545,7 @@
         <v>14000.0</v>
       </c>
       <c r="C17" t="n" s="5">
-        <v>0.0026938618433711755</v>
+        <v>0.002714756641458212</v>
       </c>
       <c r="D17" t="n" s="2">
         <v>0.0</v>
@@ -568,7 +568,7 @@
         <v>200000.0</v>
       </c>
       <c r="C18" t="n" s="5">
-        <v>0.03848374061958822</v>
+        <v>0.03878223773511732</v>
       </c>
       <c r="D18" t="n" s="2">
         <v>294.2</v>
@@ -577,10 +577,10 @@
         <v>0.04773894488602098</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>239.07976085382612</v>
+        <v>240.94915221479326</v>
       </c>
       <c r="G18" t="n" s="2">
-        <v>55.12023914617387</v>
+        <v>53.25084778520673</v>
       </c>
     </row>
     <row r="19">
@@ -591,7 +591,7 @@
         <v>160000.0</v>
       </c>
       <c r="C19" t="n" s="5">
-        <v>0.03078699249567058</v>
+        <v>0.031025790188093854</v>
       </c>
       <c r="D19" t="n" s="2">
         <v>193.11666666666702</v>
@@ -600,10 +600,10 @@
         <v>0.03133645787414038</v>
       </c>
       <c r="F19" t="n" s="2">
-        <v>191.2638086830609</v>
+        <v>192.7593217718346</v>
       </c>
       <c r="G19" t="n" s="2">
-        <v>1.8528579836061283</v>
+        <v>0.3573448948324085</v>
       </c>
     </row>
     <row r="20">
@@ -614,7 +614,7 @@
         <v>150000.0</v>
       </c>
       <c r="C20" t="n" s="5">
-        <v>0.02886280546469117</v>
+        <v>0.029086678301337987</v>
       </c>
       <c r="D20" t="n" s="2">
         <v>172.0</v>
@@ -623,10 +623,10 @@
         <v>0.027909920191691393</v>
       </c>
       <c r="F20" t="n" s="2">
-        <v>179.30982064036957</v>
+        <v>180.71186416109495</v>
       </c>
       <c r="G20" t="n" s="2">
-        <v>-7.309820640369566</v>
+        <v>-8.711864161094951</v>
       </c>
     </row>
     <row r="21">
@@ -637,7 +637,7 @@
         <v>150000.0</v>
       </c>
       <c r="C21" t="n" s="5">
-        <v>0.02886280546469117</v>
+        <v>0.029086678301337987</v>
       </c>
       <c r="D21" t="n" s="2">
         <v>198.78333333333302</v>
@@ -646,10 +646,10 @@
         <v>0.032255970748672744</v>
       </c>
       <c r="F21" t="n" s="2">
-        <v>179.30982064036957</v>
+        <v>180.71186416109495</v>
       </c>
       <c r="G21" t="n" s="2">
-        <v>19.473512692963453</v>
+        <v>18.071469172238068</v>
       </c>
     </row>
     <row r="22">
@@ -660,7 +660,7 @@
         <v>200000.0</v>
       </c>
       <c r="C22" t="n" s="5">
-        <v>0.03848374061958822</v>
+        <v>0.03878223773511732</v>
       </c>
       <c r="D22" t="n" s="2">
         <v>263.4</v>
@@ -669,10 +669,10 @@
         <v>0.04274112196797391</v>
       </c>
       <c r="F22" t="n" s="2">
-        <v>239.07976085382612</v>
+        <v>240.94915221479326</v>
       </c>
       <c r="G22" t="n" s="2">
-        <v>24.32023914617386</v>
+        <v>22.45084778520672</v>
       </c>
     </row>
     <row r="23">
@@ -683,7 +683,7 @@
         <v>300000.0</v>
       </c>
       <c r="C23" t="n" s="5">
-        <v>0.05772561092938234</v>
+        <v>0.058173356602675974</v>
       </c>
       <c r="D23" t="n" s="2">
         <v>239.8</v>
@@ -692,10 +692,10 @@
         <v>0.038911621290509284</v>
       </c>
       <c r="F23" t="n" s="2">
-        <v>358.61964128073913</v>
+        <v>361.4237283221899</v>
       </c>
       <c r="G23" t="n" s="2">
-        <v>-118.81964128073912</v>
+        <v>-121.62372832218989</v>
       </c>
     </row>
     <row r="24">
@@ -706,7 +706,7 @@
         <v>14000.0</v>
       </c>
       <c r="C24" t="n" s="5">
-        <v>0.0026938618433711755</v>
+        <v>0.002714756641458212</v>
       </c>
       <c r="D24" t="n" s="2">
         <v>0.0</v>
@@ -729,7 +729,7 @@
         <v>200000.0</v>
       </c>
       <c r="C25" t="n" s="5">
-        <v>0.03848374061958822</v>
+        <v>0.03878223773511732</v>
       </c>
       <c r="D25" t="n" s="2">
         <v>278.25</v>
@@ -738,10 +738,10 @@
         <v>0.04515078658917518</v>
       </c>
       <c r="F25" t="n" s="2">
-        <v>239.07976085382612</v>
+        <v>240.94915221479326</v>
       </c>
       <c r="G25" t="n" s="2">
-        <v>39.170239146173884</v>
+        <v>37.30084778520674</v>
       </c>
     </row>
     <row r="26">
@@ -752,7 +752,7 @@
         <v>160000.0</v>
       </c>
       <c r="C26" t="n" s="5">
-        <v>0.03078699249567058</v>
+        <v>0.031025790188093854</v>
       </c>
       <c r="D26" t="n" s="2">
         <v>221.5</v>
@@ -761,10 +761,10 @@
         <v>0.035942135595695604</v>
       </c>
       <c r="F26" t="n" s="2">
-        <v>191.2638086830609</v>
+        <v>192.7593217718346</v>
       </c>
       <c r="G26" t="n" s="2">
-        <v>30.236191316939113</v>
+        <v>28.740678228165393</v>
       </c>
     </row>
     <row r="27">
@@ -775,7 +775,7 @@
         <v>150000.0</v>
       </c>
       <c r="C27" t="n" s="5">
-        <v>0.02886280546469117</v>
+        <v>0.029086678301337987</v>
       </c>
       <c r="D27" t="n" s="2">
         <v>189.0</v>
@@ -784,10 +784,10 @@
         <v>0.030668458815288797</v>
       </c>
       <c r="F27" t="n" s="2">
-        <v>179.30982064036957</v>
+        <v>180.71186416109495</v>
       </c>
       <c r="G27" t="n" s="2">
-        <v>9.690179359630434</v>
+        <v>8.288135838905049</v>
       </c>
     </row>
     <row r="28">
@@ -798,7 +798,7 @@
         <v>170000.0</v>
       </c>
       <c r="C28" t="n" s="5">
-        <v>0.03271117952664999</v>
+        <v>0.03296490207484972</v>
       </c>
       <c r="D28" t="n" s="2">
         <v>201.8</v>
@@ -807,10 +807,10 @@
         <v>0.03274547613187979</v>
       </c>
       <c r="F28" t="n" s="2">
-        <v>203.21779672575215</v>
+        <v>204.8067793825743</v>
       </c>
       <c r="G28" t="n" s="2">
-        <v>-1.4177967257521402</v>
+        <v>-3.0067793825742797</v>
       </c>
     </row>
     <row r="29">
@@ -821,7 +821,7 @@
         <v>250000.0</v>
       </c>
       <c r="C29" t="n" s="5">
-        <v>0.04810467577448528</v>
+        <v>0.04847779716889664</v>
       </c>
       <c r="D29" t="n" s="2">
         <v>258.5</v>
@@ -830,10 +830,10 @@
         <v>0.04194601377646642</v>
       </c>
       <c r="F29" t="n" s="2">
-        <v>298.84970106728264</v>
+        <v>301.18644026849154</v>
       </c>
       <c r="G29" t="n" s="2">
-        <v>-40.34970106728264</v>
+        <v>-42.68644026849154</v>
       </c>
     </row>
     <row r="30">
@@ -844,7 +844,7 @@
         <v>300000.0</v>
       </c>
       <c r="C30" t="n" s="5">
-        <v>0.05772561092938234</v>
+        <v>0.058173356602675974</v>
       </c>
       <c r="D30" t="n" s="2">
         <v>274.9</v>
@@ -853,10 +853,10 @@
         <v>0.04460719221334863</v>
       </c>
       <c r="F30" t="n" s="2">
-        <v>358.61964128073913</v>
+        <v>361.4237283221899</v>
       </c>
       <c r="G30" t="n" s="2">
-        <v>-83.71964128073915</v>
+        <v>-86.52372832218992</v>
       </c>
     </row>
     <row r="31">
@@ -867,7 +867,7 @@
         <v>270000.0</v>
       </c>
       <c r="C31" t="n" s="5">
-        <v>0.0519530498364441</v>
+        <v>0.05235602094240838</v>
       </c>
       <c r="D31" t="n" s="2">
         <v>219.533333333333</v>
@@ -876,10 +876,10 @@
         <v>0.03562301053924016</v>
       </c>
       <c r="F31" t="n" s="2">
-        <v>322.7576771526652</v>
+        <v>325.2813554899709</v>
       </c>
       <c r="G31" t="n" s="2">
-        <v>-103.22434381933223</v>
+        <v>-105.74802215663792</v>
       </c>
     </row>
     <row r="32">
@@ -890,7 +890,7 @@
         <v>210000.0</v>
       </c>
       <c r="C32" t="n" s="5">
-        <v>0.04040792765056764</v>
+        <v>0.04072134962187318</v>
       </c>
       <c r="D32" t="n" s="2">
         <v>250.583333333333</v>
@@ -899,10 +899,10 @@
         <v>0.04066140020175189</v>
       </c>
       <c r="F32" t="n" s="2">
-        <v>251.0337488965174</v>
+        <v>252.99660982553291</v>
       </c>
       <c r="G32" t="n" s="2">
-        <v>-0.4504155631844071</v>
+        <v>-2.4132764921999126</v>
       </c>
     </row>
     <row r="33">
@@ -913,7 +913,7 @@
         <v>200000.0</v>
       </c>
       <c r="C33" t="n" s="5">
-        <v>0.03848374061958822</v>
+        <v>0.03878223773511732</v>
       </c>
       <c r="D33" t="n" s="2">
         <v>227.9</v>
@@ -922,10 +922,10 @@
         <v>0.0369806442539911</v>
       </c>
       <c r="F33" t="n" s="2">
-        <v>239.07976085382612</v>
+        <v>240.94915221479326</v>
       </c>
       <c r="G33" t="n" s="2">
-        <v>-11.17976085382611</v>
+        <v>-13.049152214793253</v>
       </c>
     </row>
     <row r="34">
@@ -933,7 +933,7 @@
         <v>31</v>
       </c>
       <c r="B34" t="n" s="3">
-        <v>5197000.0</v>
+        <v>5157000.0</v>
       </c>
       <c r="C34" t="n" s="3">
         <v>1.0</v>
@@ -945,7 +945,7 @@
         <v>1.0</v>
       </c>
       <c r="F34" t="n" s="3">
-        <v>6162.280836007368</v>
+        <v>6162.274567893339</v>
       </c>
       <c r="G34" t="n" s="3">
         <v>0.0</v>

</xml_diff>

<commit_message>
added method to create department sheet, and two columns added method to calculate daily department turnover
</commit_message>
<xml_diff>
--- a/RaportGrafików.xlsx
+++ b/RaportGrafików.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sklep" r:id="rId3" sheetId="1"/>
+    <sheet name="BieganieOXELO" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Dzień</t>
   </si>
@@ -137,13 +138,18 @@
     <numFmt numFmtId="165" formatCode="#"/>
     <numFmt numFmtId="166" formatCode="###0,00\ &quot;zł&quot;;-###0,00\ &quot;zł&quot;"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -177,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -190,6 +196,19 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -970,4 +989,392 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="11.3046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.98046875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.44921875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="s" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s" s="11">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s" s="11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="A4" t="s" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n" s="13">
+        <v>20826.061663758</v>
+      </c>
+      <c r="C4" t="n" s="12">
+        <v>0.02326934264107039</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" t="n" s="13">
+        <v>34710.10277293</v>
+      </c>
+      <c r="C5" t="n" s="12">
+        <v>0.03878223773511732</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" t="n" s="13">
+        <v>20826.061663758</v>
+      </c>
+      <c r="C6" t="n" s="12">
+        <v>0.02326934264107039</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="B7" t="n" s="13">
+        <v>20826.061663758</v>
+      </c>
+      <c r="C7" t="n" s="12">
+        <v>0.02326934264107039</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="n" s="13">
+        <v>17355.051386465</v>
+      </c>
+      <c r="C8" t="n" s="12">
+        <v>0.01939111886755866</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="B9" t="n" s="13">
+        <v>39916.6181888695</v>
+      </c>
+      <c r="C9" t="n" s="12">
+        <v>0.044599573395384916</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B10" t="n" s="13">
+        <v>1214.85359705255</v>
+      </c>
+      <c r="C10" t="n" s="12">
+        <v>0.001357378320729106</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="B11" t="n" s="13">
+        <v>30371.339926313747</v>
+      </c>
+      <c r="C11" t="n" s="12">
+        <v>0.03393445801822765</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="B12" t="n" s="13">
+        <v>29503.5873569905</v>
+      </c>
+      <c r="C12" t="n" s="12">
+        <v>0.03296490207484972</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="8">
+        <v>10</v>
+      </c>
+      <c r="B13" t="n" s="13">
+        <v>41652.123327516</v>
+      </c>
+      <c r="C13" t="n" s="12">
+        <v>0.04653868528214078</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="B14" t="n" s="13">
+        <v>1214.85359705255</v>
+      </c>
+      <c r="C14" t="n" s="12">
+        <v>0.001357378320729106</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="B15" t="n" s="13">
+        <v>46858.6387434555</v>
+      </c>
+      <c r="C15" t="n" s="12">
+        <v>0.05235602094240838</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="B16" t="n" s="13">
+        <v>52065.154159394995</v>
+      </c>
+      <c r="C16" t="n" s="12">
+        <v>0.058173356602675974</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="8">
+        <v>14</v>
+      </c>
+      <c r="B17" t="n" s="13">
+        <v>2429.7071941051</v>
+      </c>
+      <c r="C17" t="n" s="12">
+        <v>0.002714756641458212</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="8">
+        <v>15</v>
+      </c>
+      <c r="B18" t="n" s="13">
+        <v>34710.10277293</v>
+      </c>
+      <c r="C18" t="n" s="12">
+        <v>0.03878223773511732</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="B19" t="n" s="13">
+        <v>27768.082218344</v>
+      </c>
+      <c r="C19" t="n" s="12">
+        <v>0.031025790188093854</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="B20" t="n" s="13">
+        <v>26032.577079697498</v>
+      </c>
+      <c r="C20" t="n" s="12">
+        <v>0.029086678301337987</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B21" t="n" s="13">
+        <v>26032.577079697498</v>
+      </c>
+      <c r="C21" t="n" s="12">
+        <v>0.029086678301337987</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="B22" t="n" s="13">
+        <v>34710.10277293</v>
+      </c>
+      <c r="C22" t="n" s="12">
+        <v>0.03878223773511732</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="B23" t="n" s="13">
+        <v>52065.154159394995</v>
+      </c>
+      <c r="C23" t="n" s="12">
+        <v>0.058173356602675974</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="B24" t="n" s="13">
+        <v>2429.7071941051</v>
+      </c>
+      <c r="C24" t="n" s="12">
+        <v>0.002714756641458212</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="B25" t="n" s="13">
+        <v>34710.10277293</v>
+      </c>
+      <c r="C25" t="n" s="12">
+        <v>0.03878223773511732</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="B26" t="n" s="13">
+        <v>27768.082218344</v>
+      </c>
+      <c r="C26" t="n" s="12">
+        <v>0.031025790188093854</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="B27" t="n" s="13">
+        <v>26032.577079697498</v>
+      </c>
+      <c r="C27" t="n" s="12">
+        <v>0.029086678301337987</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="B28" t="n" s="13">
+        <v>29503.5873569905</v>
+      </c>
+      <c r="C28" t="n" s="12">
+        <v>0.03296490207484972</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="B29" t="n" s="13">
+        <v>43387.628466162496</v>
+      </c>
+      <c r="C29" t="n" s="12">
+        <v>0.04847779716889664</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="B30" t="n" s="13">
+        <v>52065.154159394995</v>
+      </c>
+      <c r="C30" t="n" s="12">
+        <v>0.058173356602675974</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="B31" t="n" s="13">
+        <v>46858.6387434555</v>
+      </c>
+      <c r="C31" t="n" s="12">
+        <v>0.05235602094240838</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="B32" t="n" s="13">
+        <v>36445.607911576495</v>
+      </c>
+      <c r="C32" t="n" s="12">
+        <v>0.04072134962187318</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="B33" t="n" s="13">
+        <v>34710.10277293</v>
+      </c>
+      <c r="C33" t="n" s="12">
+        <v>0.03878223773511732</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="B34" t="n" s="10">
+        <v>895000.0</v>
+      </c>
+      <c r="C34" t="n" s="10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>